<commit_message>
update chatham store and refactor with getString() instead of a generic geet()
</commit_message>
<xml_diff>
--- a/Plastic_bag_fee_stores_log.xlsx
+++ b/Plastic_bag_fee_stores_log.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sfd1z\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sfd1z\oxygen_workspace\server-application-wfc\srmobile-serverapp\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -15,7 +15,7 @@
     <sheet name="Stores for Plastic Bag Fee" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Stores for Plastic Bag Fee'!$A$1:$G$39</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Stores for Plastic Bag Fee'!$A$1:$F$39</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
   <extLst>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="62">
   <si>
     <t>Effective Date</t>
   </si>
@@ -146,12 +146,6 @@
     <t>Store Member Chain</t>
   </si>
   <si>
-    <t>Yes/NO</t>
-  </si>
-  <si>
-    <t>Yes</t>
-  </si>
-  <si>
     <t>BF80788</t>
   </si>
   <si>
@@ -213,6 +207,12 @@
   </si>
   <si>
     <t>NY starts Plastic Bag ban on 3/1/2020</t>
+  </si>
+  <si>
+    <t>Village North</t>
+  </si>
+  <si>
+    <t>Chatham</t>
   </si>
 </sst>
 </file>
@@ -292,7 +292,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -329,6 +329,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -609,22 +612,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G39"/>
+  <dimension ref="A1:F40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="G24" sqref="G24"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="E45" sqref="E45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14.5703125" customWidth="1"/>
     <col min="2" max="2" width="28.42578125" style="7" customWidth="1"/>
-    <col min="5" max="5" width="20.5703125" style="14" customWidth="1"/>
-    <col min="6" max="6" width="46.140625" customWidth="1"/>
-    <col min="7" max="7" width="66.85546875" customWidth="1"/>
+    <col min="4" max="4" width="20.5703125" style="14" customWidth="1"/>
+    <col min="5" max="5" width="46.140625" customWidth="1"/>
+    <col min="6" max="6" width="66.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
@@ -634,295 +637,271 @@
       <c r="C1" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="8" t="s">
-        <v>39</v>
-      </c>
-      <c r="E1" s="12" t="s">
+      <c r="D1" s="12" t="s">
         <v>2</v>
       </c>
+      <c r="E1" s="8" t="s">
+        <v>38</v>
+      </c>
       <c r="F1" s="8" t="s">
-        <v>38</v>
-      </c>
-      <c r="G1" s="8" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="15">
         <v>43830</v>
       </c>
       <c r="B2" s="11"/>
       <c r="C2" s="10"/>
-      <c r="D2" s="10"/>
-      <c r="E2" s="13" t="s">
-        <v>41</v>
-      </c>
+      <c r="D2" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="E2" s="10"/>
       <c r="F2" s="10"/>
-      <c r="G2" s="10"/>
-    </row>
-    <row r="3" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="15">
         <v>43830</v>
       </c>
       <c r="B3" s="11"/>
       <c r="C3" s="10"/>
-      <c r="D3" s="10"/>
-      <c r="E3" s="13" t="s">
-        <v>42</v>
-      </c>
+      <c r="D3" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="E3" s="10"/>
       <c r="F3" s="10"/>
-      <c r="G3" s="10"/>
-    </row>
-    <row r="4" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="15">
         <v>43830</v>
       </c>
       <c r="B4" s="11"/>
       <c r="C4" s="10"/>
-      <c r="D4" s="10"/>
-      <c r="E4" s="13" t="s">
-        <v>43</v>
-      </c>
+      <c r="D4" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="E4" s="10"/>
       <c r="F4" s="10"/>
-      <c r="G4" s="10"/>
-    </row>
-    <row r="5" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="15">
         <v>43830</v>
       </c>
       <c r="B5" s="11"/>
       <c r="C5" s="10"/>
-      <c r="D5" s="10"/>
-      <c r="E5" s="13" t="s">
-        <v>44</v>
-      </c>
+      <c r="D5" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="E5" s="10"/>
       <c r="F5" s="10"/>
-      <c r="G5" s="10"/>
-    </row>
-    <row r="6" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="15">
         <v>43830</v>
       </c>
       <c r="B6" s="11"/>
       <c r="C6" s="10"/>
-      <c r="D6" s="10"/>
-      <c r="E6" s="13" t="s">
-        <v>45</v>
-      </c>
+      <c r="D6" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="E6" s="10"/>
       <c r="F6" s="10"/>
-      <c r="G6" s="10"/>
-    </row>
-    <row r="7" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="15">
         <v>43830</v>
       </c>
       <c r="B7" s="11"/>
       <c r="C7" s="10"/>
-      <c r="D7" s="10"/>
-      <c r="E7" s="13" t="s">
-        <v>46</v>
-      </c>
+      <c r="D7" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="E7" s="10"/>
       <c r="F7" s="10"/>
-      <c r="G7" s="10"/>
-    </row>
-    <row r="8" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="15">
         <v>43830</v>
       </c>
       <c r="B8" s="11"/>
       <c r="C8" s="10"/>
-      <c r="D8" s="10"/>
-      <c r="E8" s="13">
+      <c r="D8" s="13">
         <v>92273195</v>
       </c>
+      <c r="E8" s="10"/>
       <c r="F8" s="10"/>
-      <c r="G8" s="10"/>
-    </row>
-    <row r="9" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="15">
         <v>43830</v>
       </c>
       <c r="B9" s="11"/>
       <c r="C9" s="10"/>
-      <c r="D9" s="10"/>
-      <c r="E9" s="13" t="s">
-        <v>47</v>
-      </c>
+      <c r="D9" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="E9" s="10"/>
       <c r="F9" s="10"/>
-      <c r="G9" s="10"/>
-    </row>
-    <row r="10" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="15">
         <v>43830</v>
       </c>
       <c r="B10" s="11"/>
       <c r="C10" s="10"/>
-      <c r="D10" s="10"/>
-      <c r="E10" s="13">
+      <c r="D10" s="13">
         <v>40583953</v>
       </c>
+      <c r="E10" s="10"/>
       <c r="F10" s="10"/>
-      <c r="G10" s="10"/>
-    </row>
-    <row r="11" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="11" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="15">
         <v>43830</v>
       </c>
       <c r="B11" s="11"/>
       <c r="C11" s="10"/>
-      <c r="D11" s="10"/>
-      <c r="E11" s="13" t="s">
-        <v>48</v>
-      </c>
+      <c r="D11" s="13" t="s">
+        <v>46</v>
+      </c>
+      <c r="E11" s="10"/>
       <c r="F11" s="10"/>
-      <c r="G11" s="10"/>
-    </row>
-    <row r="12" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="12" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="15">
         <v>43830</v>
       </c>
       <c r="B12" s="11"/>
       <c r="C12" s="10"/>
-      <c r="D12" s="10"/>
-      <c r="E12" s="13" t="s">
-        <v>49</v>
-      </c>
+      <c r="D12" s="13" t="s">
+        <v>47</v>
+      </c>
+      <c r="E12" s="10"/>
       <c r="F12" s="10"/>
-      <c r="G12" s="10"/>
-    </row>
-    <row r="13" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="13" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="15">
         <v>43830</v>
       </c>
       <c r="B13" s="11"/>
       <c r="C13" s="10"/>
-      <c r="D13" s="10"/>
-      <c r="E13" s="13" t="s">
-        <v>50</v>
-      </c>
+      <c r="D13" s="13" t="s">
+        <v>48</v>
+      </c>
+      <c r="E13" s="10"/>
       <c r="F13" s="10"/>
-      <c r="G13" s="10"/>
-    </row>
-    <row r="14" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="14" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="15">
         <v>43830</v>
       </c>
       <c r="B14" s="11"/>
       <c r="C14" s="10"/>
-      <c r="D14" s="10"/>
-      <c r="E14" s="13" t="s">
-        <v>51</v>
-      </c>
+      <c r="D14" s="13" t="s">
+        <v>49</v>
+      </c>
+      <c r="E14" s="10"/>
       <c r="F14" s="10"/>
-      <c r="G14" s="10"/>
-    </row>
-    <row r="15" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="15" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="15">
         <v>43830</v>
       </c>
       <c r="B15" s="11"/>
       <c r="C15" s="10"/>
-      <c r="D15" s="10"/>
-      <c r="E15" s="13" t="s">
-        <v>52</v>
-      </c>
+      <c r="D15" s="13" t="s">
+        <v>50</v>
+      </c>
+      <c r="E15" s="10"/>
       <c r="F15" s="10"/>
-      <c r="G15" s="10"/>
-    </row>
-    <row r="16" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="16" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="15">
         <v>43830</v>
       </c>
       <c r="B16" s="11"/>
       <c r="C16" s="10"/>
-      <c r="D16" s="10"/>
-      <c r="E16" s="13" t="s">
-        <v>53</v>
-      </c>
+      <c r="D16" s="13" t="s">
+        <v>51</v>
+      </c>
+      <c r="E16" s="10"/>
       <c r="F16" s="10"/>
-      <c r="G16" s="10"/>
-    </row>
-    <row r="17" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="17" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="15">
         <v>43830</v>
       </c>
       <c r="B17" s="11"/>
       <c r="C17" s="10"/>
-      <c r="D17" s="10"/>
-      <c r="E17" s="13" t="s">
-        <v>54</v>
-      </c>
+      <c r="D17" s="13" t="s">
+        <v>52</v>
+      </c>
+      <c r="E17" s="10"/>
       <c r="F17" s="10"/>
-      <c r="G17" s="10"/>
-    </row>
-    <row r="18" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="18" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="15">
         <v>43830</v>
       </c>
       <c r="B18" s="11"/>
       <c r="C18" s="10"/>
-      <c r="D18" s="10"/>
-      <c r="E18" s="13" t="s">
-        <v>55</v>
-      </c>
+      <c r="D18" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="E18" s="10"/>
       <c r="F18" s="10"/>
-      <c r="G18" s="10"/>
-    </row>
-    <row r="19" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="19" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="15">
         <v>43830</v>
       </c>
       <c r="B19" s="11"/>
       <c r="C19" s="10"/>
-      <c r="D19" s="10"/>
-      <c r="E19" s="13" t="s">
-        <v>56</v>
-      </c>
+      <c r="D19" s="13" t="s">
+        <v>54</v>
+      </c>
+      <c r="E19" s="10"/>
       <c r="F19" s="10"/>
-      <c r="G19" s="10"/>
-    </row>
-    <row r="20" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="20" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="15">
         <v>43830</v>
       </c>
       <c r="B20" s="11"/>
       <c r="C20" s="10"/>
-      <c r="D20" s="10"/>
-      <c r="E20" s="13" t="s">
-        <v>57</v>
-      </c>
+      <c r="D20" s="13" t="s">
+        <v>55</v>
+      </c>
+      <c r="E20" s="10"/>
       <c r="F20" s="10"/>
-      <c r="G20" s="10"/>
-    </row>
-    <row r="21" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="21" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="15">
         <v>43830</v>
       </c>
       <c r="B21" s="11"/>
       <c r="C21" s="10"/>
-      <c r="D21" s="10"/>
-      <c r="E21" s="13" t="s">
-        <v>58</v>
-      </c>
+      <c r="D21" s="13" t="s">
+        <v>56</v>
+      </c>
+      <c r="E21" s="10"/>
       <c r="F21" s="10"/>
-      <c r="G21" s="10"/>
-    </row>
-    <row r="22" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="22" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="15">
         <v>43830</v>
       </c>
       <c r="B22" s="11"/>
       <c r="C22" s="10"/>
-      <c r="D22" s="10"/>
-      <c r="E22" s="13" t="s">
-        <v>59</v>
-      </c>
-      <c r="F22" s="10"/>
-      <c r="G22" s="10" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D22" s="13" t="s">
+        <v>57</v>
+      </c>
+      <c r="E22" s="10"/>
+      <c r="F22" s="10" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>43891</v>
       </c>
@@ -932,20 +911,17 @@
       <c r="C23">
         <v>202</v>
       </c>
-      <c r="D23" t="s">
-        <v>40</v>
-      </c>
-      <c r="E23" s="14" t="s">
+      <c r="D23" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="F23" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="G23" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E23" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="F23" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>43891</v>
       </c>
@@ -955,17 +931,14 @@
       <c r="C24">
         <v>206</v>
       </c>
-      <c r="D24" t="s">
-        <v>40</v>
-      </c>
-      <c r="E24" s="14" t="s">
+      <c r="D24" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="F24" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E24" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>43891</v>
       </c>
@@ -975,17 +948,14 @@
       <c r="C25">
         <v>211</v>
       </c>
-      <c r="D25" t="s">
-        <v>40</v>
-      </c>
-      <c r="E25" s="14" t="s">
+      <c r="D25" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="F25" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E25" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>43891</v>
       </c>
@@ -995,17 +965,14 @@
       <c r="C26">
         <v>214</v>
       </c>
-      <c r="D26" t="s">
-        <v>40</v>
-      </c>
-      <c r="E26" s="14" t="s">
+      <c r="D26" s="14" t="s">
         <v>25</v>
       </c>
-      <c r="F26" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E26" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>43891</v>
       </c>
@@ -1015,17 +982,14 @@
       <c r="C27">
         <v>229</v>
       </c>
-      <c r="D27" t="s">
-        <v>40</v>
-      </c>
-      <c r="E27" s="14" t="s">
+      <c r="D27" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="F27" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E27" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>43891</v>
       </c>
@@ -1035,17 +999,14 @@
       <c r="C28">
         <v>230</v>
       </c>
-      <c r="D28" t="s">
-        <v>40</v>
-      </c>
-      <c r="E28" s="14" t="s">
+      <c r="D28" s="14" t="s">
         <v>27</v>
       </c>
-      <c r="F28" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E28" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>43891</v>
       </c>
@@ -1055,17 +1016,14 @@
       <c r="C29">
         <v>232</v>
       </c>
-      <c r="D29" t="s">
-        <v>40</v>
-      </c>
-      <c r="E29" s="13" t="s">
+      <c r="D29" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="F29" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E29" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <v>43891</v>
       </c>
@@ -1075,17 +1033,14 @@
       <c r="C30">
         <v>239</v>
       </c>
-      <c r="D30" t="s">
-        <v>40</v>
-      </c>
-      <c r="E30" s="14" t="s">
+      <c r="D30" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="F30" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E30" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <v>43891</v>
       </c>
@@ -1095,17 +1050,14 @@
       <c r="C31">
         <v>241</v>
       </c>
-      <c r="D31" t="s">
-        <v>40</v>
-      </c>
-      <c r="E31" s="14" t="s">
+      <c r="D31" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="F31" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E31" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
         <v>43891</v>
       </c>
@@ -1115,17 +1067,14 @@
       <c r="C32">
         <v>242</v>
       </c>
-      <c r="D32" t="s">
-        <v>40</v>
-      </c>
-      <c r="E32" s="14" t="s">
+      <c r="D32" s="14" t="s">
         <v>32</v>
       </c>
-      <c r="F32" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E32" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
         <v>43891</v>
       </c>
@@ -1135,17 +1084,14 @@
       <c r="C33">
         <v>250</v>
       </c>
-      <c r="D33" t="s">
-        <v>40</v>
-      </c>
-      <c r="E33" s="14" t="s">
+      <c r="D33" s="14" t="s">
         <v>33</v>
       </c>
-      <c r="F33" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E33" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
         <v>43891</v>
       </c>
@@ -1155,17 +1101,14 @@
       <c r="C34">
         <v>260</v>
       </c>
-      <c r="D34" t="s">
-        <v>40</v>
-      </c>
-      <c r="E34" s="14">
+      <c r="D34" s="14">
         <v>4326628</v>
       </c>
-      <c r="F34" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E34" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
         <v>43891</v>
       </c>
@@ -1175,17 +1118,14 @@
       <c r="C35">
         <v>263</v>
       </c>
-      <c r="D35" t="s">
-        <v>40</v>
-      </c>
-      <c r="E35" s="14" t="s">
+      <c r="D35" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="F35" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E35" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
         <v>43891</v>
       </c>
@@ -1195,17 +1135,14 @@
       <c r="C36">
         <v>267</v>
       </c>
-      <c r="D36" t="s">
-        <v>40</v>
-      </c>
-      <c r="E36" s="14" t="s">
+      <c r="D36" s="14" t="s">
         <v>35</v>
       </c>
-      <c r="F36" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E36" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
         <v>43891</v>
       </c>
@@ -1215,14 +1152,11 @@
       <c r="C37">
         <v>277</v>
       </c>
-      <c r="D37" t="s">
-        <v>40</v>
-      </c>
-      <c r="E37" s="14">
+      <c r="D37" s="14">
         <v>1492123792</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
         <v>43891</v>
       </c>
@@ -1232,14 +1166,11 @@
       <c r="C38">
         <v>278</v>
       </c>
-      <c r="D38" t="s">
-        <v>40</v>
-      </c>
-      <c r="E38" s="14" t="s">
+      <c r="D38" s="14" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
         <v>43891</v>
       </c>
@@ -1249,18 +1180,32 @@
       <c r="C39">
         <v>293</v>
       </c>
-      <c r="D39" t="s">
-        <v>40</v>
-      </c>
-      <c r="E39" s="14" t="s">
+      <c r="D39" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="F39" s="2" t="s">
-        <v>22</v>
+      <c r="E39" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A40" s="1">
+        <v>43896</v>
+      </c>
+      <c r="B40" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="C40">
+        <v>284</v>
+      </c>
+      <c r="D40" s="16">
+        <v>1420746</v>
+      </c>
+      <c r="E40" s="2" t="s">
+        <v>60</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:G39"/>
+  <autoFilter ref="A1:F39"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
remove 3 stores for the plastic bag ban
</commit_message>
<xml_diff>
--- a/Plastic_bag_fee_stores_log.xlsx
+++ b/Plastic_bag_fee_stores_log.xlsx
@@ -3,18 +3,14 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sfd1z\oxygen_workspace\server-application-wfc\srmobile-serverapp\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9600"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17076" windowHeight="5376"/>
   </bookViews>
   <sheets>
     <sheet name="Stores for Plastic Bag Fee" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="0"/>
+  <oleSize ref="A1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -303,7 +299,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.00_)"/>
   </numFmts>
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -368,6 +364,14 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <strike/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -410,7 +414,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -469,6 +473,19 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="14" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -754,7 +771,7 @@
   <dimension ref="A1:F48"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B37" sqref="B37"/>
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -842,16 +859,16 @@
       <c r="F5" s="4"/>
     </row>
     <row r="6" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="5">
-        <v>43830</v>
-      </c>
-      <c r="B6" s="26" t="s">
+      <c r="A6" s="28">
+        <v>43830</v>
+      </c>
+      <c r="B6" s="29" t="s">
         <v>76</v>
       </c>
-      <c r="C6" s="18">
+      <c r="C6" s="30">
         <v>398</v>
       </c>
-      <c r="D6" s="9" t="s">
+      <c r="D6" s="31" t="s">
         <v>49</v>
       </c>
       <c r="E6" s="4"/>
@@ -1025,16 +1042,16 @@
       <c r="F17" s="4"/>
     </row>
     <row r="18" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="5">
-        <v>43830</v>
-      </c>
-      <c r="B18" s="26" t="s">
+      <c r="A18" s="28">
+        <v>43830</v>
+      </c>
+      <c r="B18" s="29" t="s">
         <v>86</v>
       </c>
-      <c r="C18" s="18">
+      <c r="C18" s="30">
         <v>388</v>
       </c>
-      <c r="D18" s="9" t="s">
+      <c r="D18" s="31" t="s">
         <v>47</v>
       </c>
       <c r="E18" s="4"/>
@@ -1455,16 +1472,16 @@
       <c r="E43" s="7"/>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A44" s="5">
+      <c r="A44" s="28">
         <v>44021</v>
       </c>
-      <c r="B44" s="27" t="s">
+      <c r="B44" s="29" t="s">
         <v>67</v>
       </c>
-      <c r="C44" s="11">
+      <c r="C44" s="32">
         <v>399</v>
       </c>
-      <c r="D44" s="11" t="s">
+      <c r="D44" s="32" t="s">
         <v>68</v>
       </c>
       <c r="E44" s="7"/>

</xml_diff>

<commit_message>
Chore/plastic bag/remove stores (#137)
* remove 3 stores for the plastic bag ban

* update release info
</commit_message>
<xml_diff>
--- a/Plastic_bag_fee_stores_log.xlsx
+++ b/Plastic_bag_fee_stores_log.xlsx
@@ -3,18 +3,14 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sfd1z\oxygen_workspace\server-application-wfc\srmobile-serverapp\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9600"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17076" windowHeight="5376"/>
   </bookViews>
   <sheets>
     <sheet name="Stores for Plastic Bag Fee" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="0"/>
+  <oleSize ref="A1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -303,7 +299,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.00_)"/>
   </numFmts>
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -368,6 +364,14 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <strike/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -410,7 +414,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -469,6 +473,19 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="14" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -754,7 +771,7 @@
   <dimension ref="A1:F48"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B37" sqref="B37"/>
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -842,16 +859,16 @@
       <c r="F5" s="4"/>
     </row>
     <row r="6" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="5">
-        <v>43830</v>
-      </c>
-      <c r="B6" s="26" t="s">
+      <c r="A6" s="28">
+        <v>43830</v>
+      </c>
+      <c r="B6" s="29" t="s">
         <v>76</v>
       </c>
-      <c r="C6" s="18">
+      <c r="C6" s="30">
         <v>398</v>
       </c>
-      <c r="D6" s="9" t="s">
+      <c r="D6" s="31" t="s">
         <v>49</v>
       </c>
       <c r="E6" s="4"/>
@@ -1025,16 +1042,16 @@
       <c r="F17" s="4"/>
     </row>
     <row r="18" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="5">
-        <v>43830</v>
-      </c>
-      <c r="B18" s="26" t="s">
+      <c r="A18" s="28">
+        <v>43830</v>
+      </c>
+      <c r="B18" s="29" t="s">
         <v>86</v>
       </c>
-      <c r="C18" s="18">
+      <c r="C18" s="30">
         <v>388</v>
       </c>
-      <c r="D18" s="9" t="s">
+      <c r="D18" s="31" t="s">
         <v>47</v>
       </c>
       <c r="E18" s="4"/>
@@ -1455,16 +1472,16 @@
       <c r="E43" s="7"/>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A44" s="5">
+      <c r="A44" s="28">
         <v>44021</v>
       </c>
-      <c r="B44" s="27" t="s">
+      <c r="B44" s="29" t="s">
         <v>67</v>
       </c>
-      <c r="C44" s="11">
+      <c r="C44" s="32">
         <v>399</v>
       </c>
-      <c r="D44" s="11" t="s">
+      <c r="D44" s="32" t="s">
         <v>68</v>
       </c>
       <c r="E44" s="7"/>

</xml_diff>

<commit_message>
remove store Canton from the plastic bag ban
</commit_message>
<xml_diff>
--- a/Plastic_bag_fee_stores_log.xlsx
+++ b/Plastic_bag_fee_stores_log.xlsx
@@ -3,6 +3,11 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="153222"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sfd1z\oxygen_workspace\server-application-wfc\srmobile-serverapp\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="17076" windowHeight="5376"/>
   </bookViews>
@@ -10,7 +15,6 @@
     <sheet name="Stores for Plastic Bag Fee" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -771,7 +775,7 @@
   <dimension ref="A1:F48"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="A5" sqref="A5:D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -843,16 +847,16 @@
       </c>
     </row>
     <row r="5" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="5">
-        <v>43830</v>
-      </c>
-      <c r="B5" s="26" t="s">
+      <c r="A5" s="28">
+        <v>43830</v>
+      </c>
+      <c r="B5" s="29" t="s">
         <v>75</v>
       </c>
-      <c r="C5" s="18">
+      <c r="C5" s="30">
         <v>367</v>
       </c>
-      <c r="D5" s="9" t="s">
+      <c r="D5" s="31" t="s">
         <v>46</v>
       </c>
       <c r="E5" s="4"/>

</xml_diff>

<commit_message>
Chore/plastic bag/remove canton (#138)
* remove store Canton from the plastic bag ban

* update release info
</commit_message>
<xml_diff>
--- a/Plastic_bag_fee_stores_log.xlsx
+++ b/Plastic_bag_fee_stores_log.xlsx
@@ -3,6 +3,11 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="153222"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sfd1z\oxygen_workspace\server-application-wfc\srmobile-serverapp\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="17076" windowHeight="5376"/>
   </bookViews>
@@ -10,7 +15,6 @@
     <sheet name="Stores for Plastic Bag Fee" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -771,7 +775,7 @@
   <dimension ref="A1:F48"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="A5" sqref="A5:D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -843,16 +847,16 @@
       </c>
     </row>
     <row r="5" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="5">
-        <v>43830</v>
-      </c>
-      <c r="B5" s="26" t="s">
+      <c r="A5" s="28">
+        <v>43830</v>
+      </c>
+      <c r="B5" s="29" t="s">
         <v>75</v>
       </c>
-      <c r="C5" s="18">
+      <c r="C5" s="30">
         <v>367</v>
       </c>
-      <c r="D5" s="9" t="s">
+      <c r="D5" s="31" t="s">
         <v>46</v>
       </c>
       <c r="E5" s="4"/>

</xml_diff>